<commit_message>
PF-2707: bug fix (need to set Proposing Person and Proposing Date during upload); updated the taxonomy name for TCS; use the Tenant Labels in the validation messages
</commit_message>
<xml_diff>
--- a/Source/ProjectFirma.Web/Content/excel-templates/TCSProjectTracker/Pending Projects Template.xlsx
+++ b/Source/ProjectFirma.Web/Content/excel-templates/TCSProjectTracker/Pending Projects Template.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\sitkatech\projectfirma\Source\ProjectFirma.Web\Content\excel-templates\TCSProjectTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A57C41B-4293-410F-B78E-AFA68FA28666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85C94F7-1889-4767-887D-7997A2735400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10785" yWindow="2430" windowWidth="45300" windowHeight="23430" tabRatio="820" xr2:uid="{78B30058-8F2E-4265-9AEE-7F618CBAC47F}"/>
+    <workbookView xWindow="9405" yWindow="8250" windowWidth="45300" windowHeight="23430" tabRatio="820" xr2:uid="{78B30058-8F2E-4265-9AEE-7F618CBAC47F}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="19" r:id="rId1"/>
     <sheet name="Basics" sheetId="1" r:id="rId2"/>
-    <sheet name="REF - Focus Area" sheetId="6" r:id="rId3"/>
+    <sheet name="REF - Strategy" sheetId="6" r:id="rId3"/>
     <sheet name="REF - Organization" sheetId="9" r:id="rId4"/>
     <sheet name="REF - Project Primary Contact" sheetId="10" r:id="rId5"/>
   </sheets>
@@ -265,6 +265,12 @@
     </r>
   </si>
   <si>
+    <t>Use this template to upload new pending projects to the TCS Project Tracker in bulk.</t>
+  </si>
+  <si>
+    <t>Strategy</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -287,11 +293,8 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-See the "REF - Focus Area" tab for a list of valid options</t>
-    </r>
-  </si>
-  <si>
-    <t>Focus Area</t>
+See the "REF - Strategy" tab for a list of valid options</t>
+    </r>
   </si>
   <si>
     <r>
@@ -310,7 +313,7 @@
 &gt;The following fields are required:
       -Project Name 
       -Description
-      -Focus Area
+      -Strategy
       -Project Stage
       -Planning/Design Start Year
       -Implementation Start Year</t>
@@ -344,9 +347,6 @@
 &gt;If the Project Stage is "Completed", then the completion year is required
 &gt;If Latitude and Longitude are blank, a note explaining why the location has not been provided must be added.</t>
     </r>
-  </si>
-  <si>
-    <t>Use this template to upload new pending projects to the TCS Project Tracker in bulk.</t>
   </si>
 </sst>
 </file>
@@ -875,7 +875,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -886,7 +886,7 @@
     </row>
     <row r="6" spans="1:1" ht="255" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
@@ -1008,7 +1008,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>21</v>
@@ -1121,7 +1121,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AC3070F3-E37E-4A18-8963-03C6178C4E0F}">
           <x14:formula1>
-            <xm:f>'REF - Focus Area'!$A$2:$A$1048576</xm:f>
+            <xm:f>'REF - Strategy'!$A$2:$A$1048576</xm:f>
           </x14:formula1>
           <xm:sqref>C4:C1048576</xm:sqref>
         </x14:dataValidation>

</xml_diff>